<commit_message>
Add DC questionnaire question.
</commit_message>
<xml_diff>
--- a/Coverage Survey/Burkina Faso/IVM+ALB/cs1_village.xlsx
+++ b/Coverage Survey/Burkina Faso/IVM+ALB/cs1_village.xlsx
@@ -392,10 +392,10 @@
     <t>nom_grappe</t>
   </si>
   <si>
-    <t>bf_Coverage-mars_2020-lf-village</t>
-  </si>
-  <si>
     <t>(BF - Mars 2020) Couv ALB+IVM FL - 1. Formulaire Village</t>
+  </si>
+  <si>
+    <t>bf_Coverage_mars_2020_1lf_village</t>
   </si>
 </sst>
 </file>
@@ -2336,7 +2336,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2359,10 +2359,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
         <v>110</v>
-      </c>
-      <c r="B2" t="s">
-        <v>109</v>
       </c>
       <c r="C2" s="17">
         <v>20200305</v>

</xml_diff>

<commit_message>
🎨 Improve BF coverage survey forms.
</commit_message>
<xml_diff>
--- a/Coverage Survey/Burkina Faso/IVM+ALB/cs1_village.xlsx
+++ b/Coverage Survey/Burkina Faso/IVM+ALB/cs1_village.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <author>HP</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="108">
   <si>
     <t>form_title</t>
   </si>
@@ -198,15 +198,6 @@
   </si>
   <si>
     <t>Sélectionner de code d'équipe (1 à 5) comme les autres enquête</t>
-  </si>
-  <si>
-    <t>select_one code_equipe</t>
-  </si>
-  <si>
-    <t>code_equipe</t>
-  </si>
-  <si>
-    <t>Code Equipe</t>
   </si>
   <si>
     <t>csps_list</t>
@@ -402,7 +393,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -503,13 +494,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -563,7 +547,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -618,12 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -917,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -970,58 +948,56 @@
       </c>
       <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="1:11" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+    <row r="2" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
       <c r="I2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="23"/>
-    </row>
-    <row r="3" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14" t="s">
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>100</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -1031,138 +1007,119 @@
       <c r="I4" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="9" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="16"/>
+    </row>
+    <row r="7" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>29</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="I8" s="7"/>
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="8"/>
+      <c r="A9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1172,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1200,15 +1157,15 @@
         <v>43</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>107</v>
+        <v>45</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>46</v>
+      <c r="A2" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>32</v>
@@ -1216,11 +1173,11 @@
       <c r="C2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="22"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>46</v>
+      <c r="A3" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>33</v>
@@ -1228,11 +1185,11 @@
       <c r="C3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>46</v>
+      <c r="A4" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>34</v>
@@ -1240,11 +1197,11 @@
       <c r="C4" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>46</v>
+      <c r="A5" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>35</v>
@@ -1252,89 +1209,97 @@
       <c r="C5" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="18"/>
+    </row>
+    <row r="6" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="18"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="18"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="18"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="18"/>
+      <c r="B6" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="11"/>
+      <c r="A10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>42</v>
@@ -1342,13 +1307,13 @@
     </row>
     <row r="13" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>42</v>
@@ -1356,13 +1321,13 @@
     </row>
     <row r="14" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>42</v>
@@ -1370,13 +1335,13 @@
     </row>
     <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>52</v>
+        <v>45</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>42</v>
@@ -1384,13 +1349,13 @@
     </row>
     <row r="16" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>42</v>
@@ -1398,13 +1363,13 @@
     </row>
     <row r="17" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>42</v>
@@ -1412,350 +1377,350 @@
     </row>
     <row r="18" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="10">
+        <v>1</v>
+      </c>
+      <c r="C19" s="10">
+        <v>1</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" s="10">
-        <v>1</v>
-      </c>
-      <c r="C23" s="10">
-        <v>1</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12" t="s">
-        <v>49</v>
+        <v>104</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B29">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C29">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C30">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B31">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C31">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B32">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C32">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B33">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C33">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B34">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C34">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B35">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C35">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B36">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C36">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B37">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C37">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E37" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B38">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C38">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B39">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C39">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E39" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B40">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C40">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B41">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C41">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B42">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C42">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E42" t="s">
         <v>54</v>
@@ -1763,13 +1728,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B43">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C43">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E43" t="s">
         <v>54</v>
@@ -1777,13 +1742,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B44">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C44">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E44" t="s">
         <v>55</v>
@@ -1791,533 +1756,477 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B45">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C45">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B46">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C46">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B47">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C47">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B48">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C48">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E48" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B49">
-        <v>27</v>
-      </c>
-      <c r="C49">
-        <v>27</v>
-      </c>
-      <c r="E49" t="s">
-        <v>58</v>
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
+        <v>59</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B50">
-        <v>28</v>
-      </c>
-      <c r="C50">
-        <v>28</v>
-      </c>
-      <c r="E50" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B51">
-        <v>29</v>
-      </c>
-      <c r="C51">
-        <v>29</v>
-      </c>
-      <c r="E51" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="B51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" t="s">
+        <v>61</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B52">
-        <v>30</v>
-      </c>
-      <c r="C52">
-        <v>30</v>
-      </c>
-      <c r="E52" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+      <c r="B52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" t="s">
+        <v>62</v>
+      </c>
+      <c r="F52">
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F54">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="C55" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F55">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="F56">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="C57" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F57">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F58">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F59">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>69</v>
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" t="s">
+        <v>70</v>
       </c>
       <c r="F60">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="C61" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F61">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C62" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F62">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F63">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C64" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F64">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C65" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F65">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C66" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F66">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F67">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C68" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F68">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C69" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F69">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C70" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F70">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C71" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F71">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B72" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C72" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F72">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C73" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F73">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C74" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F74">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C75" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F75">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C76" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F76">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F77">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B78" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C78" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F78">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B79" t="s">
-        <v>88</v>
-      </c>
-      <c r="C79" t="s">
-        <v>88</v>
-      </c>
-      <c r="F79">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B80" t="s">
-        <v>97</v>
-      </c>
-      <c r="C80" t="s">
-        <v>89</v>
-      </c>
-      <c r="F80">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B81" t="s">
-        <v>90</v>
-      </c>
-      <c r="C81" t="s">
-        <v>90</v>
-      </c>
-      <c r="F81">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B82" t="s">
-        <v>91</v>
-      </c>
-      <c r="C82" t="s">
-        <v>91</v>
-      </c>
-      <c r="F82">
         <v>30</v>
       </c>
     </row>
@@ -2335,7 +2244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2359,10 +2268,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C2" s="17">
         <v>20200305</v>

</xml_diff>